<commit_message>
adding additoinal geography data
</commit_message>
<xml_diff>
--- a/interactive_map_men.xlsx
+++ b/interactive_map_men.xlsx
@@ -1129,7 +1129,7 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>KEN</t>
+          <t>Kenya</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">

</xml_diff>